<commit_message>
Project Plan progress updated, Suvarna tasks tab updated
</commit_message>
<xml_diff>
--- a/CSV_Uploader_Project_Plan.xlsx
+++ b/CSV_Uploader_Project_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suvarnajoshi\Documents\ByteAcademy\MyProjects\PyQt_Projects\Csv_Uploader_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2242013-B273-418D-8EDA-9BD5CFFCEF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F1D171-408D-4DBA-A90C-22CFF9C82F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Github</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Learnt command prompt GIT commands</t>
   </si>
   <si>
-    <t>Guided on command prompt GIT commands</t>
-  </si>
-  <si>
     <t>Created Folder Structure &amp; Checked in files to Github</t>
   </si>
   <si>
@@ -152,6 +149,28 @@
   </si>
   <si>
     <t>Added User Stories on Github</t>
+  </si>
+  <si>
+    <t>Created &amp; Added this Project plan file to repository</t>
+  </si>
+  <si>
+    <t>Added the test folder structure to repo with sample test file</t>
+  </si>
+  <si>
+    <t>Learnt PyQt5 
+Calculator App</t>
+  </si>
+  <si>
+    <t>Learnt pytest &amp; unittest 
+(Python Unit test)</t>
+  </si>
+  <si>
+    <t>Guided on command prompt 
+GIT commands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code for login dialog window (frontend) 
+added to view.py </t>
   </si>
 </sst>
 </file>
@@ -206,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +256,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -461,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -476,24 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,6 +530,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -835,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27167FBF-5415-45B1-A6B3-569F9CE78ED2}">
   <dimension ref="A3:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,38 +891,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" s="21" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18">
+    <row r="4" spans="1:11" s="15" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="12">
         <v>43773</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="13">
         <v>43774</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="13">
         <v>43775</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="13">
         <v>43776</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="13">
         <v>43777</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="13">
         <v>43778</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="13">
         <v>43779</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="13">
         <v>43780</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="13">
         <v>43781</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="13">
         <v>43782</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="14">
         <v>43783</v>
       </c>
     </row>
@@ -894,10 +932,10 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="10"/>
@@ -917,8 +955,8 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -944,8 +982,8 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
         <v>23</v>
@@ -965,15 +1003,15 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -982,8 +1020,8 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -995,8 +1033,8 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1008,8 +1046,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1021,8 +1059,8 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1034,8 +1072,8 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1047,8 +1085,8 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1060,8 +1098,8 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1073,8 +1111,8 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="17"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1093,15 +1131,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177830E0-DBE4-43DA-B808-268D22DB5622}">
   <dimension ref="A4:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1115,40 +1152,40 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="18">
+      <c r="A5" s="12">
         <v>43773</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="13">
         <v>43774</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="13">
         <v>43775</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="13">
         <v>43776</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="13">
         <v>43777</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="13">
         <v>43778</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="13">
         <v>43779</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="13">
         <v>43780</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="13">
         <v>43781</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="13">
         <v>43782</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="14">
         <v>43783</v>
       </c>
-      <c r="L5" s="21"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
@@ -1156,10 +1193,10 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="10"/>
@@ -1168,10 +1205,10 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1179,8 +1216,8 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1195,10 +1232,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1206,8 +1243,8 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
         <v>23</v>
@@ -1218,34 +1255,38 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="33" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="33" t="s">
+        <v>7</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1257,8 +1298,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1270,8 +1311,8 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1283,8 +1324,8 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1296,8 +1337,8 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1309,8 +1350,8 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1322,8 +1363,8 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="16"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1335,8 +1376,8 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="17"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1368,7 +1409,7 @@
   <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,12 +1418,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1411,7 +1452,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1421,10 +1462,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1478,40 +1519,40 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
-      <c r="L3" s="21"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -1519,10 +1560,10 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="10"/>
@@ -1531,60 +1572,60 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>28</v>
+      <c r="A6" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>29</v>
+      <c r="A7" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>31</v>
+      <c r="A8" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1596,8 +1637,8 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1609,8 +1650,8 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1622,8 +1663,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1635,8 +1676,8 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1660,12 +1701,13 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1679,40 +1721,40 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
-      <c r="L3" s="21"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -1720,10 +1762,10 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="10"/>
@@ -1731,72 +1773,82 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2"/>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3"/>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="3"/>
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1808,8 +1860,8 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1821,8 +1873,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1834,8 +1886,8 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1878,40 +1930,40 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
-      <c r="L3" s="21"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -1919,10 +1971,10 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="10"/>
@@ -1931,69 +1983,69 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>29</v>
+      <c r="A6" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2005,8 +2057,8 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2018,8 +2070,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2031,8 +2083,8 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -2056,7 +2108,7 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2075,40 +2127,40 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
-      <c r="L3" s="21"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -2116,10 +2168,10 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="10"/>
@@ -2128,56 +2180,56 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>29</v>
+      <c r="A6" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2189,8 +2241,8 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2202,8 +2254,8 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2215,8 +2267,8 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2228,8 +2280,8 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>

</xml_diff>

<commit_message>
Updated project plan xls with today's update
</commit_message>
<xml_diff>
--- a/CSV_Uploader_Project_Plan.xlsx
+++ b/CSV_Uploader_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suvarnajoshi\Documents\ByteAcademy\MyProjects\PyQt_Projects\Csv_Uploader_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F1D171-408D-4DBA-A90C-22CFF9C82F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E198C-6421-4576-AD19-B01A40878311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>Github</t>
   </si>
@@ -171,6 +171,43 @@
   <si>
     <t xml:space="preserve">Code for login dialog window (frontend) 
 added to view.py </t>
+  </si>
+  <si>
+    <t>Add appropriate 
+methods/functions 
+Add doc strings
+to the functions</t>
+  </si>
+  <si>
+    <t>Added LearningModule folder 
+with tutorial files for 
+Logging in Python and 
+a quick guide for 
+GIT commands</t>
+  </si>
+  <si>
+    <t>Took a session on 
+Logging in Python</t>
+  </si>
+  <si>
+    <t>Added function definitions, 
+doc strings &amp; to-dos for the 
+controller &amp; model files</t>
+  </si>
+  <si>
+    <t>Code View.py 
+for Login</t>
+  </si>
+  <si>
+    <t>Code Controller.py 
+for Login</t>
+  </si>
+  <si>
+    <t>Code Controller.py 
+for implementing Logging</t>
+  </si>
+  <si>
+    <t>Add User Stories</t>
   </si>
 </sst>
 </file>
@@ -225,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,12 +299,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -492,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -554,9 +585,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +906,7 @@
   <dimension ref="A3:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,7 +914,8 @@
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -953,7 +986,9 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="26"/>
       <c r="G6" s="29"/>
@@ -980,7 +1015,9 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="20" t="s">
+        <v>3</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="26"/>
       <c r="G7" s="29"/>
@@ -1001,7 +1038,9 @@
         <v>6</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="26"/>
       <c r="G8" s="29"/>
@@ -1015,10 +1054,12 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="26"/>
       <c r="G9" s="29"/>
@@ -1027,11 +1068,13 @@
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="26"/>
       <c r="G10" s="29"/>
@@ -1132,13 +1175,14 @@
   <dimension ref="A4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1211,10 +1255,12 @@
       <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="26"/>
       <c r="G7" s="29"/>
@@ -1238,10 +1284,12 @@
       <c r="B8" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="34" t="s">
+        <v>3</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="26"/>
       <c r="G8" s="29"/>
@@ -1264,7 +1312,9 @@
       <c r="C9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="26"/>
       <c r="G9" s="29"/>
@@ -1281,9 +1331,11 @@
         <v>7</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="26"/>
       <c r="G10" s="29"/>
@@ -1292,11 +1344,13 @@
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="26"/>
       <c r="G11" s="29"/>
@@ -1701,14 +1755,14 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -1780,7 +1834,9 @@
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="26"/>
@@ -1790,14 +1846,16 @@
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="26"/>
@@ -1814,7 +1872,9 @@
       <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="26"/>

</xml_diff>

<commit_message>
Updated project status & my project assignment update
</commit_message>
<xml_diff>
--- a/CSV_Uploader_Project_Plan.xlsx
+++ b/CSV_Uploader_Project_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamding/Desktop/byteproject/Csv_Uploader_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suvarnajoshi\Documents\ByteAcademy\MyProjects\PyQt_Projects\Csv_Uploader_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ED21FD-DDE4-7B4E-AE15-0BFC135942A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00633BD5-ECE2-4BD3-B8AF-B525F6B3D553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" activeTab="7" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>Github</t>
   </si>
@@ -217,6 +217,112 @@
   </si>
   <si>
     <t>learnt a bit about logging in python</t>
+  </si>
+  <si>
+    <t>Shared Knowledge 
+- SQLAlchemy
+- PostgreSQL
+- pgAdmin GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coded model.py
+</t>
+  </si>
+  <si>
+    <t>Coded send_csv() 
+in controller.py</t>
+  </si>
+  <si>
+    <t>Research SQLAlchemy
+PostgreSQL</t>
+  </si>
+  <si>
+    <t>Research 
+SQLAlchemy
+PostgreSQL</t>
+  </si>
+  <si>
+    <t>Research 
+PyQt5</t>
+  </si>
+  <si>
+    <t>Research 
+Logging in Python</t>
+  </si>
+  <si>
+    <t>Research
+&amp; shared knowledge
+for setting a new DB user account which could be used as a common one for project</t>
+  </si>
+  <si>
+    <t>DB Setup to be 
+done by all</t>
+  </si>
+  <si>
+    <t>Code View.py for 
+browsing file</t>
+  </si>
+  <si>
+    <t>Code Controller.py 
+for csv validation</t>
+  </si>
+  <si>
+    <t>Code Controller.py 
+for updating db with csv data</t>
+  </si>
+  <si>
+    <t>Code 
+test_controller.py 
+for login validation</t>
+  </si>
+  <si>
+    <t>Code 
+test_controller.py 
+for csv validation</t>
+  </si>
+  <si>
+    <t>Code 
+test_controller.py 
+for send_csv</t>
+  </si>
+  <si>
+    <t>Code View.py 
+to show/hide buttons 
+dinamically</t>
+  </si>
+  <si>
+    <t>Beautify the
+frontend</t>
+  </si>
+  <si>
+    <t>Any Additional 
+functionalities 
+to be added</t>
+  </si>
+  <si>
+    <t>Implement 
+Logout functionality</t>
+  </si>
+  <si>
+    <t>Review 
+Documentation</t>
+  </si>
+  <si>
+    <t>Work on 
+Presentation files</t>
+  </si>
+  <si>
+    <t>Research Packaging</t>
+  </si>
+  <si>
+    <t>Packaging 
+to be done</t>
+  </si>
+  <si>
+    <t>Test Packaging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB path </t>
   </si>
 </sst>
 </file>
@@ -309,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -528,11 +634,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -600,6 +715,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,188 +1036,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27167FBF-5415-45B1-A6B3-569F9CE78ED2}">
-  <dimension ref="A3:K16"/>
+  <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:11" s="15" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="30" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="F6" s="31"/>
       <c r="G6" s="34"/>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
+      <c r="H6" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>57</v>
+      </c>
       <c r="F7" s="31"/>
       <c r="G7" s="34"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>24</v>
+      <c r="H7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
+    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>58</v>
+      </c>
       <c r="F8" s="31"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="H8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>37</v>
-      </c>
+    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>59</v>
+      </c>
       <c r="F9" s="31"/>
       <c r="G9" s="34"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="62.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="31"/>
       <c r="G10" s="34"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1108,7 +1276,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1121,7 +1289,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1134,7 +1302,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1147,36 +1315,23 @@
       <c r="J14" s="2"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F5:F16"/>
-    <mergeCell ref="G5:G16"/>
+    <mergeCell ref="F4:F15"/>
+    <mergeCell ref="G4:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1184,185 +1339,245 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177830E0-DBE4-43DA-B808-268D22DB5622}">
-  <dimension ref="A4:L20"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12">
         <v>43773</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B3" s="13">
         <v>43774</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C3" s="13">
         <v>43775</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D3" s="13">
         <v>43776</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E3" s="13">
         <v>43777</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F3" s="13">
         <v>43778</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G3" s="13">
         <v>43779</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H3" s="13">
         <v>43780</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I3" s="13">
         <v>43781</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J3" s="13">
         <v>43782</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K3" s="14">
         <v>43783</v>
       </c>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="30" t="s">
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D5" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E5" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="F7" s="31"/>
       <c r="G7" s="34"/>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>58</v>
+      </c>
       <c r="F8" s="31"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>24</v>
+      <c r="H8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="2"/>
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>59</v>
+      </c>
       <c r="F9" s="31"/>
       <c r="G9" s="34"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="10" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="31"/>
       <c r="G10" s="34"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="31"/>
       <c r="G11" s="34"/>
@@ -1371,7 +1586,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1384,7 +1599,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1397,7 +1612,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1410,61 +1625,35 @@
       <c r="J14" s="2"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F6:F17"/>
-    <mergeCell ref="G6:G17"/>
+    <mergeCell ref="F4:F15"/>
+    <mergeCell ref="G4:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1472,40 +1661,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72BEA59-A2B4-45AE-B79A-FDFFA572A736}">
-  <dimension ref="A2:A9"/>
+  <dimension ref="A2:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1518,16 +1712,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
@@ -1535,7 +1729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1543,7 +1737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1551,7 +1745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1569,22 +1763,22 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>43773</v>
       </c>
@@ -1620,7 +1814,7 @@
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1637,7 +1831,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
@@ -1652,7 +1846,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
@@ -1667,7 +1861,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>28</v>
       </c>
@@ -1682,7 +1876,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
@@ -1697,7 +1891,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1710,7 +1904,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1723,7 +1917,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1736,7 +1930,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="112.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1749,7 +1943,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -1767,26 +1961,28 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>43773</v>
       </c>
@@ -1822,7 +2018,7 @@
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1839,7 +2035,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>35</v>
       </c>
@@ -1849,8 +2045,12 @@
       <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F5" s="31"/>
       <c r="G5" s="34"/>
       <c r="H5" s="4"/>
@@ -1858,7 +2058,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>29</v>
       </c>
@@ -1868,8 +2068,12 @@
       <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F6" s="31"/>
       <c r="G6" s="34"/>
       <c r="H6" s="2"/>
@@ -1877,7 +2081,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>28</v>
       </c>
@@ -1888,7 +2092,9 @@
         <v>40</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F7" s="31"/>
       <c r="G7" s="34"/>
       <c r="H7" s="2"/>
@@ -1896,12 +2102,16 @@
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+    <row r="8" spans="1:12" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>53</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="31"/>
@@ -1911,7 +2121,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>36</v>
@@ -1926,9 +2136,11 @@
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1939,7 +2151,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1952,7 +2164,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1965,7 +2177,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -1986,22 +2198,22 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>43773</v>
       </c>
@@ -2037,7 +2249,7 @@
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2054,7 +2266,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
@@ -2069,7 +2281,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>28</v>
       </c>
@@ -2084,7 +2296,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -2097,7 +2309,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -2110,7 +2322,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2123,7 +2335,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2136,7 +2348,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2149,7 +2361,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2162,7 +2374,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -2179,26 +2391,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F77CE66-450A-48BC-AF0C-EDEBFA4B78A0}">
   <dimension ref="A2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="34.77734375" customWidth="1"/>
     <col min="4" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>43773</v>
       </c>
@@ -2234,7 +2446,7 @@
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2251,7 +2463,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
@@ -2270,7 +2482,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>28</v>
       </c>
@@ -2287,7 +2499,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2300,7 +2512,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2313,7 +2525,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2326,7 +2538,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2339,7 +2551,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2352,7 +2564,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2365,7 +2577,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added new tab FutureEnhancementsPlan
</commit_message>
<xml_diff>
--- a/CSV_Uploader_Project_Plan.xlsx
+++ b/CSV_Uploader_Project_Plan.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suvarnajoshi\Documents\ByteAcademy\MyProjects\PyQt_Projects\Csv_Uploader_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00633BD5-ECE2-4BD3-B8AF-B525F6B3D553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669DA6E6-B6D8-4879-9BB0-C964A6040F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{CBB71D51-1D17-4A98-9576-F49BC28C6369}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Plan_Execution_Update" sheetId="2" r:id="rId2"/>
     <sheet name="Things to Remember" sheetId="3" r:id="rId3"/>
     <sheet name="AdditionsToPlan" sheetId="4" r:id="rId4"/>
-    <sheet name="Aditya" sheetId="5" r:id="rId5"/>
-    <sheet name="Suvarna" sheetId="6" r:id="rId6"/>
-    <sheet name="Sanju" sheetId="7" r:id="rId7"/>
-    <sheet name="Tamdin" sheetId="8" r:id="rId8"/>
+    <sheet name="FutureEnhancementsPlan" sheetId="9" r:id="rId5"/>
+    <sheet name="Aditya" sheetId="5" r:id="rId6"/>
+    <sheet name="Suvarna" sheetId="6" r:id="rId7"/>
+    <sheet name="Sanju" sheetId="7" r:id="rId8"/>
+    <sheet name="Tamdin" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Github</t>
   </si>
@@ -323,6 +324,30 @@
   </si>
   <si>
     <t xml:space="preserve">DB path </t>
+  </si>
+  <si>
+    <t>Future Enhancements plan</t>
+  </si>
+  <si>
+    <t>Admin frontend can be added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin frontend can include </t>
+  </si>
+  <si>
+    <t>b) Update user functionalities</t>
+  </si>
+  <si>
+    <t>a) Add user functionalities</t>
+  </si>
+  <si>
+    <t>c) Delete user functionalities</t>
+  </si>
+  <si>
+    <t>d) Add database setup details</t>
+  </si>
+  <si>
+    <t>e) Add table &amp; columns setup details</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177830E0-DBE4-43DA-B808-268D22DB5622}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -1756,6 +1781,79 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54346CBB-FC02-4D6D-9FFE-782D4EB795A2}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="57.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC21BFE-6A2C-4103-BFDF-C3FD694BF3E0}">
   <dimension ref="A2:L13"/>
   <sheetViews>
@@ -1956,7 +2054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FC322-7CEA-402E-8E54-FA36DDA002ED}">
   <dimension ref="A2:L13"/>
   <sheetViews>
@@ -2190,7 +2288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8FCC78-EE0F-493A-BE01-C8B4FF9DF8FE}">
   <dimension ref="A2:L13"/>
   <sheetViews>
@@ -2387,7 +2485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F77CE66-450A-48BC-AF0C-EDEBFA4B78A0}">
   <dimension ref="A2:L13"/>
   <sheetViews>

</xml_diff>